<commit_message>
revising the adding columns based on the title as well
</commit_message>
<xml_diff>
--- a/test/table_1.xlsx
+++ b/test/table_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,12 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Regression</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>API</t>
+          <t>new_regression</t>
         </is>
       </c>
     </row>
@@ -502,10 +497,7 @@
           <t>https://link.springer.com/article/10.1007/s11219-021-09579-6</t>
         </is>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -538,10 +530,7 @@
           <t>https://onlinelibrary.wiley.com/doi/abs/10.1155/2021/2912240</t>
         </is>
       </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -574,10 +563,7 @@
           <t>https://ieeexplore.ieee.org/abstract/document/9564098/</t>
         </is>
       </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -610,10 +596,7 @@
           <t>https://doi.org/10.1145/3524481.3527217</t>
         </is>
       </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -646,10 +629,7 @@
           <t>https://doi.org/10.1002/smr.2452</t>
         </is>
       </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -682,12 +662,9 @@
           <t>https://ieeexplore.ieee.org/abstract/document/8990249/</t>
         </is>
       </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>FALSE</t>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>TRUE</t>
         </is>
       </c>
     </row>
@@ -718,10 +695,7 @@
           <t>https://ieeexplore.ieee.org/abstract/document/8387249/</t>
         </is>
       </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -754,10 +728,7 @@
           <t>https://www.sciencedirect.com/science/article/pii/S0167739X19302614</t>
         </is>
       </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -790,10 +761,7 @@
           <t>https://www.researchgate.net/profile/Luigi-Lavazza/publication/366958305_ICSEA_2021_The_Sixteenth_International_Conference_on_Software_Engineering_Advances/links/63bb2e19c3c99660ebdc4ca9/ICSEA-2021-The-Sixteenth-International-Conference-on-Software-Engineering-Advances.pdf#page=99</t>
         </is>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
@@ -826,10 +794,7 @@
           <t>https://doi.org/10.1109/SOSE58276.2023.00013</t>
         </is>
       </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>

</xml_diff>